<commit_message>
curs 4 si 5
</commit_message>
<xml_diff>
--- a/curs03/CursBNR.xlsx
+++ b/curs03/CursBNR.xlsx
@@ -606,104 +606,104 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>29.11.2022</t>
+          <t>06.12.2022</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.1941</v>
+        <v>3.1421</v>
       </c>
       <c r="D2" t="n">
-        <v>2.5147</v>
+        <v>2.5117</v>
       </c>
       <c r="E2" t="n">
-        <v>3.5228</v>
+        <v>3.4338</v>
       </c>
       <c r="F2" t="n">
-        <v>4.989</v>
+        <v>4.9667</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2021</v>
+        <v>0.2019</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6614</v>
+        <v>0.6605</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1929</v>
+        <v>0.1902</v>
       </c>
       <c r="J2" t="n">
-        <v>4.9184</v>
+        <v>4.9126</v>
       </c>
       <c r="K2" t="n">
-        <v>5.6933</v>
+        <v>5.6911</v>
       </c>
       <c r="L2" t="n">
-        <v>1.2093</v>
+        <v>1.1838</v>
       </c>
       <c r="M2" t="n">
-        <v>3.4339</v>
+        <v>3.4228</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2427</v>
+        <v>0.2374</v>
       </c>
       <c r="O2" t="n">
-        <v>0.4759</v>
+        <v>0.47</v>
       </c>
       <c r="P2" t="n">
-        <v>1.0503</v>
+        <v>1.0454</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0776</v>
+        <v>0.074</v>
       </c>
       <c r="R2" t="n">
-        <v>0.4516</v>
+        <v>0.451</v>
       </c>
       <c r="S2" t="n">
-        <v>0.2543</v>
+        <v>0.2511</v>
       </c>
       <c r="T2" t="n">
-        <v>4.7383</v>
+        <v>4.6804</v>
       </c>
       <c r="U2" t="n">
-        <v>0.2793</v>
+        <v>0.2696</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8831</v>
+        <v>0.8863</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6612</v>
+        <v>0.6688</v>
       </c>
       <c r="X2" t="n">
-        <v>0.058</v>
+        <v>0.0567</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.3572</v>
+        <v>0.354</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.2485</v>
+        <v>0.2378</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.958</v>
+        <v>2.9584</v>
       </c>
       <c r="AB2" t="n">
         <v>0.0419</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.1289</v>
+        <v>0.1266</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.2901</v>
+        <v>1.2743</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.6514</v>
+        <v>0.6502</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.1339</v>
+        <v>0.1334</v>
       </c>
       <c r="AG2" t="n">
-        <v>267.3958</v>
+        <v>266.7598</v>
       </c>
       <c r="AH2" t="n">
-        <v>6.227</v>
+        <v>6.1981</v>
       </c>
     </row>
     <row r="3">
@@ -712,104 +712,104 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>28.11.2022</t>
+          <t>05.12.2022</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.1556</v>
+        <v>3.1778</v>
       </c>
       <c r="D3" t="n">
-        <v>2.5189</v>
+        <v>2.5159</v>
       </c>
       <c r="E3" t="n">
-        <v>3.5027</v>
+        <v>3.4784</v>
       </c>
       <c r="F3" t="n">
-        <v>4.9892</v>
+        <v>4.9903</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2023</v>
+        <v>0.202</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6625</v>
+        <v>0.6616</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1912</v>
+        <v>0.1899</v>
       </c>
       <c r="J3" t="n">
-        <v>4.9266</v>
+        <v>4.9207</v>
       </c>
       <c r="K3" t="n">
-        <v>5.6863</v>
+        <v>5.7178</v>
       </c>
       <c r="L3" t="n">
-        <v>1.2063</v>
+        <v>1.1975</v>
       </c>
       <c r="M3" t="n">
-        <v>3.4163</v>
+        <v>3.4523</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2447</v>
+        <v>0.2383</v>
       </c>
       <c r="O3" t="n">
-        <v>0.4757</v>
+        <v>0.4773</v>
       </c>
       <c r="P3" t="n">
-        <v>1.0521</v>
+        <v>1.0479</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.07729999999999999</v>
+        <v>0.075</v>
       </c>
       <c r="R3" t="n">
-        <v>0.453</v>
+        <v>0.4524</v>
       </c>
       <c r="S3" t="n">
-        <v>0.2526</v>
+        <v>0.2507</v>
       </c>
       <c r="T3" t="n">
-        <v>4.7043</v>
+        <v>4.6726</v>
       </c>
       <c r="U3" t="n">
-        <v>0.2754</v>
+        <v>0.2711</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8696</v>
+        <v>0.8952</v>
       </c>
       <c r="W3" t="n">
-        <v>0.654</v>
+        <v>0.6716</v>
       </c>
       <c r="X3" t="n">
-        <v>0.0577</v>
+        <v>0.0571</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.3529</v>
+        <v>0.3599</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.2435</v>
+        <v>0.2392</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.9308</v>
+        <v>2.9901</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.042</v>
+        <v>0.0419</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.128</v>
+        <v>0.1265</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.2808</v>
+        <v>1.2721</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.6526999999999999</v>
+        <v>0.6515</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1323</v>
+        <v>0.1346</v>
       </c>
       <c r="AG3" t="n">
-        <v>266.5349</v>
+        <v>269.7555</v>
       </c>
       <c r="AH3" t="n">
-        <v>6.1995</v>
+        <v>6.2057</v>
       </c>
     </row>
     <row r="4">
@@ -818,104 +818,104 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>25.11.2022</t>
+          <t>02.12.2022</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3.1913</v>
+        <v>3.1935</v>
       </c>
       <c r="D4" t="n">
-        <v>2.5181</v>
+        <v>2.5205</v>
       </c>
       <c r="E4" t="n">
-        <v>3.5438</v>
+        <v>3.486</v>
       </c>
       <c r="F4" t="n">
-        <v>5.012</v>
+        <v>5.0142</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2021</v>
+        <v>0.2023</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6623</v>
+        <v>0.6629</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1924</v>
+        <v>0.1907</v>
       </c>
       <c r="J4" t="n">
-        <v>4.925</v>
+        <v>4.9297</v>
       </c>
       <c r="K4" t="n">
-        <v>5.7274</v>
+        <v>5.7419</v>
       </c>
       <c r="L4" t="n">
-        <v>1.2003</v>
+        <v>1.2044</v>
       </c>
       <c r="M4" t="n">
-        <v>3.395</v>
+        <v>3.4938</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2453</v>
+        <v>0.2417</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4776</v>
+        <v>0.4803</v>
       </c>
       <c r="P4" t="n">
-        <v>1.0504</v>
+        <v>1.0539</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.078</v>
+        <v>0.0755</v>
       </c>
       <c r="R4" t="n">
-        <v>0.4545</v>
+        <v>0.4537</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2537</v>
+        <v>0.2516</v>
       </c>
       <c r="T4" t="n">
-        <v>4.7278</v>
+        <v>4.6851</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2765</v>
+        <v>0.2705</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8885</v>
+        <v>0.9036</v>
       </c>
       <c r="W4" t="n">
-        <v>0.6598000000000001</v>
+        <v>0.667</v>
       </c>
       <c r="X4" t="n">
-        <v>0.0579</v>
+        <v>0.0576</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3558</v>
+        <v>0.3612</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2439</v>
+        <v>0.2446</v>
       </c>
       <c r="AA4" t="n">
-        <v>2.9524</v>
+        <v>2.9969</v>
       </c>
       <c r="AB4" t="n">
         <v>0.042</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.128</v>
+        <v>0.1273</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.2872</v>
+        <v>1.2756</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.6525</v>
+        <v>0.6529</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.1321</v>
+        <v>0.1348</v>
       </c>
       <c r="AG4" t="n">
-        <v>266.4903</v>
+        <v>271.1673</v>
       </c>
       <c r="AH4" t="n">
-        <v>6.2192</v>
+        <v>6.219</v>
       </c>
     </row>
     <row r="5">
@@ -924,104 +924,104 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24.11.2022</t>
+          <t>29.11.2022</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.1966</v>
+        <v>3.1941</v>
       </c>
       <c r="D5" t="n">
-        <v>2.5211</v>
+        <v>2.5147</v>
       </c>
       <c r="E5" t="n">
-        <v>3.5514</v>
+        <v>3.5228</v>
       </c>
       <c r="F5" t="n">
-        <v>5.0256</v>
+        <v>4.989</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2025</v>
+        <v>0.2021</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6631</v>
+        <v>0.6614</v>
       </c>
       <c r="I5" t="n">
-        <v>0.193</v>
+        <v>0.1929</v>
       </c>
       <c r="J5" t="n">
-        <v>4.9309</v>
+        <v>4.9184</v>
       </c>
       <c r="K5" t="n">
-        <v>5.7413</v>
+        <v>5.6933</v>
       </c>
       <c r="L5" t="n">
-        <v>1.1883</v>
+        <v>1.2093</v>
       </c>
       <c r="M5" t="n">
-        <v>3.4276</v>
+        <v>3.4339</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2479</v>
+        <v>0.2427</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4761</v>
+        <v>0.4759</v>
       </c>
       <c r="P5" t="n">
-        <v>1.0493</v>
+        <v>1.0503</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.07820000000000001</v>
+        <v>0.0776</v>
       </c>
       <c r="R5" t="n">
-        <v>0.4527</v>
+        <v>0.4516</v>
       </c>
       <c r="S5" t="n">
-        <v>0.2544</v>
+        <v>0.2543</v>
       </c>
       <c r="T5" t="n">
-        <v>4.739</v>
+        <v>4.7383</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2788</v>
+        <v>0.2793</v>
       </c>
       <c r="V5" t="n">
-        <v>0.8842</v>
+        <v>0.8831</v>
       </c>
       <c r="W5" t="n">
-        <v>0.6633</v>
+        <v>0.6612</v>
       </c>
       <c r="X5" t="n">
         <v>0.058</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.3564</v>
+        <v>0.3572</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.2451</v>
+        <v>0.2485</v>
       </c>
       <c r="AA5" t="n">
-        <v>2.9656</v>
+        <v>2.958</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.042</v>
+        <v>0.0419</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1283</v>
+        <v>0.1289</v>
       </c>
       <c r="AD5" t="n">
-        <v>1.2902</v>
+        <v>1.2901</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.6539</v>
+        <v>0.6514</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.1325</v>
+        <v>0.1339</v>
       </c>
       <c r="AG5" t="n">
-        <v>267.5475</v>
+        <v>267.3958</v>
       </c>
       <c r="AH5" t="n">
-        <v>6.2373</v>
+        <v>6.227</v>
       </c>
     </row>
     <row r="6">
@@ -1030,104 +1030,104 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23.11.2022</t>
+          <t>28.11.2022</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.1826</v>
+        <v>3.1556</v>
       </c>
       <c r="D6" t="n">
-        <v>2.525</v>
+        <v>2.5189</v>
       </c>
       <c r="E6" t="n">
-        <v>3.5731</v>
+        <v>3.5027</v>
       </c>
       <c r="F6" t="n">
-        <v>5.0285</v>
+        <v>4.9892</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2028</v>
+        <v>0.2023</v>
       </c>
       <c r="H6" t="n">
-        <v>0.664</v>
+        <v>0.6625</v>
       </c>
       <c r="I6" t="n">
-        <v>0.195</v>
+        <v>0.1912</v>
       </c>
       <c r="J6" t="n">
-        <v>4.9385</v>
+        <v>4.9266</v>
       </c>
       <c r="K6" t="n">
-        <v>5.7102</v>
+        <v>5.6863</v>
       </c>
       <c r="L6" t="n">
-        <v>1.2168</v>
+        <v>1.2063</v>
       </c>
       <c r="M6" t="n">
-        <v>3.3875</v>
+        <v>3.4163</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2502</v>
+        <v>0.2447</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4761</v>
+        <v>0.4757</v>
       </c>
       <c r="P6" t="n">
-        <v>1.0516</v>
+        <v>1.0521</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.079</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="R6" t="n">
-        <v>0.4523</v>
+        <v>0.453</v>
       </c>
       <c r="S6" t="n">
-        <v>0.2573</v>
+        <v>0.2526</v>
       </c>
       <c r="T6" t="n">
-        <v>4.7923</v>
+        <v>4.7043</v>
       </c>
       <c r="U6" t="n">
-        <v>0.2783</v>
+        <v>0.2754</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8942</v>
+        <v>0.8696</v>
       </c>
       <c r="W6" t="n">
-        <v>0.6695</v>
+        <v>0.654</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0586</v>
+        <v>0.0577</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.3542</v>
+        <v>0.3529</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.2468</v>
+        <v>0.2435</v>
       </c>
       <c r="AA6" t="n">
-        <v>2.9566</v>
+        <v>2.9308</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.0421</v>
+        <v>0.042</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.1298</v>
+        <v>0.128</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.3047</v>
+        <v>1.2808</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.6548</v>
+        <v>0.6526999999999999</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.1322</v>
+        <v>0.1323</v>
       </c>
       <c r="AG6" t="n">
-        <v>267.605</v>
+        <v>266.5349</v>
       </c>
       <c r="AH6" t="n">
-        <v>6.2701</v>
+        <v>6.1995</v>
       </c>
     </row>
     <row r="7">
@@ -1136,104 +1136,104 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>22.11.2022</t>
+          <t>25.11.2022</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.1828</v>
+        <v>3.1913</v>
       </c>
       <c r="D7" t="n">
-        <v>2.5182</v>
+        <v>2.5181</v>
       </c>
       <c r="E7" t="n">
-        <v>3.5761</v>
+        <v>3.5438</v>
       </c>
       <c r="F7" t="n">
-        <v>5.0192</v>
+        <v>5.012</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2023</v>
+        <v>0.2021</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6622</v>
+        <v>0.6623</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1953</v>
+        <v>0.1924</v>
       </c>
       <c r="J7" t="n">
-        <v>4.9253</v>
+        <v>4.925</v>
       </c>
       <c r="K7" t="n">
-        <v>5.6838</v>
+        <v>5.7274</v>
       </c>
       <c r="L7" t="n">
-        <v>1.2047</v>
+        <v>1.2003</v>
       </c>
       <c r="M7" t="n">
-        <v>3.3901</v>
+        <v>3.395</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2509</v>
+        <v>0.2453</v>
       </c>
       <c r="O7" t="n">
-        <v>0.4701</v>
+        <v>0.4776</v>
       </c>
       <c r="P7" t="n">
-        <v>1.0467</v>
+        <v>1.0504</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.079</v>
+        <v>0.078</v>
       </c>
       <c r="R7" t="n">
-        <v>0.449</v>
+        <v>0.4545</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2573</v>
+        <v>0.2537</v>
       </c>
       <c r="T7" t="n">
-        <v>4.7918</v>
+        <v>4.7278</v>
       </c>
       <c r="U7" t="n">
-        <v>0.2774</v>
+        <v>0.2765</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9006</v>
+        <v>0.8885</v>
       </c>
       <c r="W7" t="n">
-        <v>0.6715</v>
+        <v>0.6598000000000001</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0587</v>
+        <v>0.0579</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.354</v>
+        <v>0.3558</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.2452</v>
+        <v>0.2439</v>
       </c>
       <c r="AA7" t="n">
-        <v>2.9465</v>
+        <v>2.9524</v>
       </c>
       <c r="AB7" t="n">
         <v>0.042</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.1297</v>
+        <v>0.128</v>
       </c>
       <c r="AD7" t="n">
-        <v>1.3046</v>
+        <v>1.2872</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.6529</v>
+        <v>0.6525</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.1326</v>
+        <v>0.1321</v>
       </c>
       <c r="AG7" t="n">
-        <v>269.1826</v>
+        <v>266.4903</v>
       </c>
       <c r="AH7" t="n">
-        <v>6.2652</v>
+        <v>6.2192</v>
       </c>
     </row>
     <row r="8">
@@ -1242,104 +1242,104 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21.11.2022</t>
+          <t>24.11.2022</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>3.1966</v>
       </c>
       <c r="D8" t="n">
-        <v>2.5266</v>
+        <v>2.5211</v>
       </c>
       <c r="E8" t="n">
-        <v>3.5959</v>
+        <v>3.5514</v>
       </c>
       <c r="F8" t="n">
-        <v>5.0346</v>
+        <v>5.0256</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2029</v>
+        <v>0.2025</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6643</v>
+        <v>0.6631</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1971</v>
+        <v>0.193</v>
       </c>
       <c r="J8" t="n">
-        <v>4.9417</v>
+        <v>4.9309</v>
       </c>
       <c r="K8" t="n">
-        <v>5.704</v>
+        <v>5.7413</v>
       </c>
       <c r="L8" t="n">
-        <v>1.206</v>
+        <v>1.1883</v>
       </c>
       <c r="M8" t="n">
-        <v>3.4074</v>
+        <v>3.4276</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2486</v>
+        <v>0.2479</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4707</v>
+        <v>0.4761</v>
       </c>
       <c r="P8" t="n">
-        <v>1.0509</v>
+        <v>1.0493</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0795</v>
+        <v>0.07820000000000001</v>
       </c>
       <c r="R8" t="n">
-        <v>0.4497</v>
+        <v>0.4527</v>
       </c>
       <c r="S8" t="n">
-        <v>0.2592</v>
+        <v>0.2544</v>
       </c>
       <c r="T8" t="n">
-        <v>4.8287</v>
+        <v>4.739</v>
       </c>
       <c r="U8" t="n">
-        <v>0.2773</v>
+        <v>0.2788</v>
       </c>
       <c r="V8" t="n">
-        <v>0.897</v>
+        <v>0.8842</v>
       </c>
       <c r="W8" t="n">
-        <v>0.6738</v>
+        <v>0.6633</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0591</v>
+        <v>0.058</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.3554</v>
+        <v>0.3564</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.2476</v>
+        <v>0.2451</v>
       </c>
       <c r="AA8" t="n">
-        <v>2.9546</v>
+        <v>2.9656</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.0421</v>
+        <v>0.042</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1307</v>
+        <v>0.1283</v>
       </c>
       <c r="AD8" t="n">
-        <v>1.3146</v>
+        <v>1.2902</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.6551</v>
+        <v>0.6539</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.1333</v>
+        <v>0.1325</v>
       </c>
       <c r="AG8" t="n">
-        <v>270.3308</v>
+        <v>267.5475</v>
       </c>
       <c r="AH8" t="n">
-        <v>6.2992</v>
+        <v>6.2373</v>
       </c>
     </row>
     <row r="9">
@@ -1348,104 +1348,104 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18.11.2022</t>
+          <t>23.11.2022</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3.2026</v>
+        <v>3.1826</v>
       </c>
       <c r="D9" t="n">
-        <v>2.5267</v>
+        <v>2.525</v>
       </c>
       <c r="E9" t="n">
-        <v>3.5742</v>
+        <v>3.5731</v>
       </c>
       <c r="F9" t="n">
-        <v>5.0066</v>
+        <v>5.0285</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2029</v>
+        <v>0.2028</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6644</v>
+        <v>0.664</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1942</v>
+        <v>0.195</v>
       </c>
       <c r="J9" t="n">
-        <v>4.9418</v>
+        <v>4.9385</v>
       </c>
       <c r="K9" t="n">
-        <v>5.6799</v>
+        <v>5.7102</v>
       </c>
       <c r="L9" t="n">
-        <v>1.2105</v>
+        <v>1.2168</v>
       </c>
       <c r="M9" t="n">
-        <v>3.4071</v>
+        <v>3.3875</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2492</v>
+        <v>0.2502</v>
       </c>
       <c r="O9" t="n">
-        <v>0.472</v>
+        <v>0.4761</v>
       </c>
       <c r="P9" t="n">
-        <v>1.0512</v>
+        <v>1.0516</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0789</v>
+        <v>0.079</v>
       </c>
       <c r="R9" t="n">
-        <v>0.4497</v>
+        <v>0.4523</v>
       </c>
       <c r="S9" t="n">
-        <v>0.2558</v>
+        <v>0.2573</v>
       </c>
       <c r="T9" t="n">
-        <v>4.7618</v>
+        <v>4.7923</v>
       </c>
       <c r="U9" t="n">
-        <v>0.2756</v>
+        <v>0.2783</v>
       </c>
       <c r="V9" t="n">
-        <v>0.878</v>
+        <v>0.8942</v>
       </c>
       <c r="W9" t="n">
-        <v>0.6693</v>
+        <v>0.6695</v>
       </c>
       <c r="X9" t="n">
-        <v>0.0583</v>
+        <v>0.0586</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.3559</v>
+        <v>0.3542</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.2451</v>
+        <v>0.2468</v>
       </c>
       <c r="AA9" t="n">
-        <v>2.9472</v>
+        <v>2.9566</v>
       </c>
       <c r="AB9" t="n">
         <v>0.0421</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.129</v>
+        <v>0.1298</v>
       </c>
       <c r="AD9" t="n">
-        <v>1.2964</v>
+        <v>1.3047</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.6555</v>
+        <v>0.6548</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.1334</v>
+        <v>0.1322</v>
       </c>
       <c r="AG9" t="n">
-        <v>270.2902</v>
+        <v>267.605</v>
       </c>
       <c r="AH9" t="n">
-        <v>6.2535</v>
+        <v>6.2701</v>
       </c>
     </row>
     <row r="10">
@@ -1454,104 +1454,104 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17.11.2022</t>
+          <t>22.11.2022</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.1784</v>
+        <v>3.1828</v>
       </c>
       <c r="D10" t="n">
-        <v>2.519</v>
+        <v>2.5182</v>
       </c>
       <c r="E10" t="n">
-        <v>3.563</v>
+        <v>3.5761</v>
       </c>
       <c r="F10" t="n">
-        <v>5.0162</v>
+        <v>5.0192</v>
       </c>
       <c r="G10" t="n">
-        <v>0.202</v>
+        <v>0.2023</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6623</v>
+        <v>0.6622</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1947</v>
+        <v>0.1953</v>
       </c>
       <c r="J10" t="n">
-        <v>4.9267</v>
+        <v>4.9253</v>
       </c>
       <c r="K10" t="n">
-        <v>5.6466</v>
+        <v>5.6838</v>
       </c>
       <c r="L10" t="n">
-        <v>1.1912</v>
+        <v>1.2047</v>
       </c>
       <c r="M10" t="n">
-        <v>3.405</v>
+        <v>3.3901</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2473</v>
+        <v>0.2509</v>
       </c>
       <c r="O10" t="n">
-        <v>0.4703</v>
+        <v>0.4701</v>
       </c>
       <c r="P10" t="n">
-        <v>1.0476</v>
+        <v>1.0467</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0789</v>
+        <v>0.079</v>
       </c>
       <c r="R10" t="n">
-        <v>0.4497</v>
+        <v>0.449</v>
       </c>
       <c r="S10" t="n">
-        <v>0.2558</v>
+        <v>0.2573</v>
       </c>
       <c r="T10" t="n">
-        <v>4.764</v>
+        <v>4.7918</v>
       </c>
       <c r="U10" t="n">
-        <v>0.2726</v>
+        <v>0.2774</v>
       </c>
       <c r="V10" t="n">
-        <v>0.8822</v>
+        <v>0.9006</v>
       </c>
       <c r="W10" t="n">
-        <v>0.6661</v>
+        <v>0.6715</v>
       </c>
       <c r="X10" t="n">
-        <v>0.0583</v>
+        <v>0.0587</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.3534</v>
+        <v>0.354</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.2455</v>
+        <v>0.2452</v>
       </c>
       <c r="AA10" t="n">
-        <v>2.9043</v>
+        <v>2.9465</v>
       </c>
       <c r="AB10" t="n">
         <v>0.042</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.1296</v>
+        <v>0.1297</v>
       </c>
       <c r="AD10" t="n">
-        <v>1.297</v>
+        <v>1.3046</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.6533</v>
+        <v>0.6529</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.1324</v>
+        <v>0.1326</v>
       </c>
       <c r="AG10" t="n">
-        <v>269.9403</v>
+        <v>269.1826</v>
       </c>
       <c r="AH10" t="n">
-        <v>6.2427</v>
+        <v>6.2652</v>
       </c>
     </row>
     <row r="11">
@@ -1560,104 +1560,104 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16.11.2022</t>
+          <t>21.11.2022</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.2015</v>
+        <v>3.1966</v>
       </c>
       <c r="D11" t="n">
-        <v>2.516</v>
+        <v>2.5266</v>
       </c>
       <c r="E11" t="n">
-        <v>3.5626</v>
+        <v>3.5959</v>
       </c>
       <c r="F11" t="n">
-        <v>5.0226</v>
+        <v>5.0346</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2022</v>
+        <v>0.2029</v>
       </c>
       <c r="H11" t="n">
-        <v>0.6615</v>
+        <v>0.6643</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1929</v>
+        <v>0.1971</v>
       </c>
       <c r="J11" t="n">
-        <v>4.9209</v>
+        <v>4.9417</v>
       </c>
       <c r="K11" t="n">
-        <v>5.6277</v>
+        <v>5.704</v>
       </c>
       <c r="L11" t="n">
-        <v>1.2098</v>
+        <v>1.206</v>
       </c>
       <c r="M11" t="n">
-        <v>3.3881</v>
+        <v>3.4074</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2466</v>
+        <v>0.2486</v>
       </c>
       <c r="O11" t="n">
-        <v>0.4752</v>
+        <v>0.4707</v>
       </c>
       <c r="P11" t="n">
-        <v>1.0467</v>
+        <v>1.0509</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0779</v>
+        <v>0.0795</v>
       </c>
       <c r="R11" t="n">
-        <v>0.4531</v>
+        <v>0.4497</v>
       </c>
       <c r="S11" t="n">
-        <v>0.2535</v>
+        <v>0.2592</v>
       </c>
       <c r="T11" t="n">
-        <v>4.7176</v>
+        <v>4.8287</v>
       </c>
       <c r="U11" t="n">
-        <v>0.2741</v>
+        <v>0.2773</v>
       </c>
       <c r="V11" t="n">
-        <v>0.8846000000000001</v>
+        <v>0.897</v>
       </c>
       <c r="W11" t="n">
-        <v>0.6666</v>
+        <v>0.6738</v>
       </c>
       <c r="X11" t="n">
-        <v>0.0581</v>
+        <v>0.0591</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.357</v>
+        <v>0.3554</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.2443</v>
+        <v>0.2476</v>
       </c>
       <c r="AA11" t="n">
-        <v>2.9179</v>
+        <v>2.9546</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.042</v>
+        <v>0.0421</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1279</v>
+        <v>0.1307</v>
       </c>
       <c r="AD11" t="n">
-        <v>1.2844</v>
+        <v>1.3146</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.6523</v>
+        <v>0.6551</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.1326</v>
+        <v>0.1333</v>
       </c>
       <c r="AG11" t="n">
-        <v>270.4325</v>
+        <v>270.3308</v>
       </c>
       <c r="AH11" t="n">
-        <v>6.2104</v>
+        <v>6.2992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>